<commit_message>
Update of Assemble Program #1
</commit_message>
<xml_diff>
--- a/AssemblePrograms/Instructions Program One.xlsx
+++ b/AssemblePrograms/Instructions Program One.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="157">
   <si>
     <t>MEMORY ADDRESS</t>
   </si>
@@ -38,9 +38,6 @@
     <t>HALT</t>
   </si>
   <si>
-    <t>AMR R3, 0, POS 9</t>
-  </si>
-  <si>
     <t>START</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>LDR R0,0, POS16</t>
   </si>
   <si>
-    <t>AMR R0, 0, POS9</t>
-  </si>
-  <si>
     <t>Load index to memory</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>else, go keep adding numbers in the array</t>
   </si>
   <si>
-    <t>Start</t>
-  </si>
-  <si>
     <t>JCC CC(1), 0, POS 7, 1</t>
   </si>
   <si>
@@ -320,9 +311,6 @@
     <t>LDR R2,0, POS26</t>
   </si>
   <si>
-    <t>AMR R3, 0, POS9</t>
-  </si>
-  <si>
     <t xml:space="preserve">STORE IX 1  </t>
   </si>
   <si>
@@ -383,9 +371,6 @@
     <t>1500, 1500</t>
   </si>
   <si>
-    <t>store number close</t>
-  </si>
-  <si>
     <t>Add 1 to index number</t>
   </si>
   <si>
@@ -396,16 +381,143 @@
   </si>
   <si>
     <t>LDX IX 3, POS11</t>
+  </si>
+  <si>
+    <t>start phase 5</t>
+  </si>
+  <si>
+    <t>LDR R0,IX2, 1</t>
+  </si>
+  <si>
+    <t>STX IX 3, POS11</t>
+  </si>
+  <si>
+    <t>LDR R1,0, POS27</t>
+  </si>
+  <si>
+    <t>STR R1,0, POS11</t>
+  </si>
+  <si>
+    <t>SMR R0, 0, IX 3, 1</t>
+  </si>
+  <si>
+    <t>Substract numbers</t>
+  </si>
+  <si>
+    <t>Put substract result in R0</t>
+  </si>
+  <si>
+    <t>continue iterating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000, 100 </t>
+  </si>
+  <si>
+    <t>LDX IX 1, POS7</t>
+  </si>
+  <si>
+    <t>Index 1 initialize</t>
+  </si>
+  <si>
+    <t>JCC CC(1), IX1, 1</t>
+  </si>
+  <si>
+    <t>LDX IX2, POS11</t>
+  </si>
+  <si>
+    <t>Replace IX2 with IX3</t>
+  </si>
+  <si>
+    <t>AIR R3, 0, 1</t>
+  </si>
+  <si>
+    <t>AIR R0, 0, 1</t>
+  </si>
+  <si>
+    <t>AIR R1, 0, 1</t>
+  </si>
+  <si>
+    <t>LDA R2, 0, 20</t>
+  </si>
+  <si>
+    <t>Initialize array flag limit</t>
+  </si>
+  <si>
+    <t>TRR R2, R3</t>
+  </si>
+  <si>
+    <t>Is array limit?</t>
+  </si>
+  <si>
+    <t>JCC CC(3), 0, POS30, 1</t>
+  </si>
+  <si>
+    <t>If array, go to print function</t>
+  </si>
+  <si>
+    <t>JMA 0, POS31, 1</t>
+  </si>
+  <si>
+    <t>If not, continue iterating</t>
+  </si>
+  <si>
+    <t>Go to continue iterating or check limit</t>
+  </si>
+  <si>
+    <t>If array limit, go to print function</t>
+  </si>
+  <si>
+    <t>Load index 3 number to index 3</t>
+  </si>
+  <si>
+    <t>LDX, IX2, POS 27</t>
+  </si>
+  <si>
+    <t>Load IX2 to its pos</t>
+  </si>
+  <si>
+    <t>LDR, R0, POS 27</t>
+  </si>
+  <si>
+    <t>Load index to resgister 0</t>
+  </si>
+  <si>
+    <t>SMR, R0, POS 19</t>
+  </si>
+  <si>
+    <t>Substract 500 from memory pos to get address number</t>
+  </si>
+  <si>
+    <t>STR, R0, POS 29</t>
+  </si>
+  <si>
+    <t>Put mem position of the closest number in memory</t>
+  </si>
+  <si>
+    <t>store mempost of close number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -431,11 +543,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,19 +830,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
@@ -742,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -751,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -759,10 +873,10 @@
         <v>499</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -771,13 +885,13 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -785,10 +899,10 @@
         <v>500</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>7</v>
@@ -797,7 +911,7 @@
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -808,10 +922,10 @@
         <v>501</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -820,7 +934,7 @@
         <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -831,19 +945,16 @@
         <v>502</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>9</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -854,10 +965,10 @@
         <v>503</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -871,25 +982,25 @@
         <v>504</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7">
-        <v>1000</v>
+        <v>9</v>
+      </c>
+      <c r="I7" t="s">
+        <v>128</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -897,10 +1008,10 @@
         <v>505</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -909,16 +1020,16 @@
         <v>499</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -926,25 +1037,25 @@
         <v>506</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9">
         <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -952,10 +1063,10 @@
         <v>507</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E10">
         <v>14</v>
@@ -969,19 +1080,19 @@
         <v>508</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E11">
         <v>15</v>
       </c>
       <c r="F11">
-        <v>2000</v>
+        <v>520</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -989,16 +1100,16 @@
         <v>509</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E12">
         <v>16</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1006,10 +1117,10 @@
         <v>510</v>
       </c>
       <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
         <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
       </c>
       <c r="E13">
         <v>17</v>
@@ -1023,19 +1134,19 @@
         <v>511</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E14">
         <v>18</v>
       </c>
       <c r="F14">
-        <v>2100</v>
+        <v>540</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1043,16 +1154,16 @@
         <v>512</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>19</v>
       </c>
-      <c r="F15" t="s">
-        <v>51</v>
+      <c r="F15">
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1060,16 +1171,16 @@
         <v>513</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16">
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1080,16 +1191,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17">
         <v>21</v>
       </c>
       <c r="F17">
-        <v>2199</v>
+        <v>558</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1097,19 +1208,19 @@
         <v>515</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E18">
         <v>22</v>
       </c>
       <c r="F18">
-        <v>2099</v>
+        <v>539</v>
       </c>
       <c r="G18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1117,61 +1228,61 @@
         <v>23</v>
       </c>
       <c r="F19">
-        <v>2250</v>
+        <v>580</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2000</v>
+        <v>520</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20">
         <v>24</v>
       </c>
       <c r="F20">
-        <v>2260</v>
+        <v>600</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2001</v>
+        <v>521</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E21">
         <v>25</v>
       </c>
       <c r="F21">
-        <v>2200</v>
+        <v>560</v>
       </c>
       <c r="G21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2002</v>
+        <v>522</v>
       </c>
       <c r="B22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" t="s">
         <v>34</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
       </c>
       <c r="E22">
         <v>26</v>
@@ -1182,117 +1293,129 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2003</v>
+        <v>523</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23">
         <v>27</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2004</v>
+        <v>524</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24">
         <v>28</v>
       </c>
       <c r="F24">
-        <v>2300</v>
+        <v>620</v>
       </c>
       <c r="G24" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2005</v>
+        <v>525</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E25">
         <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2006</v>
+        <v>526</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E26">
         <v>30</v>
       </c>
+      <c r="F26">
+        <v>700</v>
+      </c>
+      <c r="G26" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2007</v>
+        <v>527</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E27">
         <v>31</v>
       </c>
+      <c r="F27">
+        <v>631</v>
+      </c>
+      <c r="G27" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2008</v>
+        <v>528</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2009</v>
+        <v>529</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2099</v>
+        <v>539</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31">
         <v>100</v>
@@ -1303,13 +1426,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2100</v>
+        <v>540</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32">
         <v>1001</v>
@@ -1320,13 +1443,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2101</v>
+        <v>541</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E33">
         <v>1002</v>
@@ -1334,13 +1457,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2102</v>
+        <v>542</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E34">
         <v>1003</v>
@@ -1348,13 +1471,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2103</v>
+        <v>543</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E35">
         <v>1004</v>
@@ -1362,13 +1485,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2104</v>
+        <v>544</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E36">
         <v>1005</v>
@@ -1376,13 +1499,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2105</v>
+        <v>545</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E37">
         <v>1006</v>
@@ -1390,13 +1513,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2106</v>
+        <v>546</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E38">
         <v>1007</v>
@@ -1404,13 +1527,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2107</v>
+        <v>547</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E39">
         <v>1008</v>
@@ -1418,13 +1541,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2108</v>
+        <v>548</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E40">
         <v>1009</v>
@@ -1432,13 +1555,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2109</v>
+        <v>549</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E41">
         <v>1010</v>
@@ -1446,13 +1569,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>2110</v>
+        <v>550</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E42">
         <v>1011</v>
@@ -1460,13 +1583,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2111</v>
+        <v>551</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E43">
         <v>1012</v>
@@ -1474,13 +1597,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>2112</v>
+        <v>552</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E44">
         <v>1013</v>
@@ -1488,13 +1611,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>2113</v>
+        <v>553</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E45">
         <v>1014</v>
@@ -1502,13 +1625,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>2114</v>
+        <v>554</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E46">
         <v>1015</v>
@@ -1516,13 +1639,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>2115</v>
+        <v>555</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E47">
         <v>1016</v>
@@ -1535,13 +1658,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>2198</v>
+        <v>558</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E49">
         <v>1018</v>
@@ -1549,13 +1672,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2199</v>
+        <v>559</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E50">
         <v>1019</v>
@@ -1563,13 +1686,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>2200</v>
+        <v>560</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E51">
         <v>1020</v>
@@ -1577,24 +1700,24 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2201</v>
+        <v>561</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>2202</v>
+        <v>562</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E53">
         <v>1501</v>
@@ -1602,13 +1725,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>2203</v>
+        <v>563</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E54">
         <v>1502</v>
@@ -1616,13 +1739,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>2204</v>
+        <v>564</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E55">
         <v>1503</v>
@@ -1630,13 +1753,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>2205</v>
+        <v>565</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E56">
         <v>1504</v>
@@ -1649,13 +1772,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2250</v>
+        <v>580</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E58">
         <v>1506</v>
@@ -1663,13 +1786,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>2251</v>
+        <v>581</v>
       </c>
       <c r="B59" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C59" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E59">
         <v>1507</v>
@@ -1677,13 +1800,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>2252</v>
+        <v>582</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C60" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E60">
         <v>1508</v>
@@ -1691,13 +1814,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>2253</v>
+        <v>583</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E61">
         <v>1509</v>
@@ -1705,13 +1828,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>2254</v>
+        <v>584</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C62" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E62">
         <v>1510</v>
@@ -1724,13 +1847,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>2260</v>
+        <v>600</v>
       </c>
       <c r="B64" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E64">
         <v>1512</v>
@@ -1738,13 +1861,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>2261</v>
+        <v>601</v>
       </c>
       <c r="B65" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C65" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E65">
         <v>1513</v>
@@ -1752,13 +1875,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>2262</v>
+        <v>602</v>
       </c>
       <c r="B66" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C66" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E66">
         <v>1514</v>
@@ -1766,13 +1889,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>2263</v>
+        <v>603</v>
       </c>
       <c r="B67" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" t="s">
         <v>34</v>
-      </c>
-      <c r="C67" t="s">
-        <v>36</v>
       </c>
       <c r="E67">
         <v>1515</v>
@@ -1780,13 +1903,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>2264</v>
+        <v>604</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E68">
         <v>1516</v>
@@ -1794,13 +1917,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>2265</v>
+        <v>605</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C69" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E69">
         <v>1517</v>
@@ -1808,13 +1931,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>2266</v>
+        <v>606</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E70">
         <v>1518</v>
@@ -1822,13 +1945,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>2267</v>
+        <v>607</v>
       </c>
       <c r="B71" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" t="s">
         <v>34</v>
-      </c>
-      <c r="C71" t="s">
-        <v>36</v>
       </c>
       <c r="E71">
         <v>1519</v>
@@ -1836,13 +1959,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>2268</v>
+        <v>608</v>
       </c>
       <c r="B72" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C72" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E72">
         <v>1520</v>
@@ -1850,159 +1973,408 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>2269</v>
+        <v>609</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>2270</v>
+        <v>610</v>
       </c>
       <c r="B74" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C74" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>2271</v>
+        <v>611</v>
       </c>
       <c r="B75" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C75" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>2272</v>
+        <v>612</v>
       </c>
       <c r="B76" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>2273</v>
+        <v>613</v>
       </c>
       <c r="B77" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C77" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>2300</v>
+        <v>620</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C79" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>2301</v>
+        <v>621</v>
       </c>
       <c r="B80" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C80" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>2302</v>
+        <v>622</v>
       </c>
       <c r="B81" t="s">
+        <v>111</v>
+      </c>
+      <c r="C81" t="s">
+        <v>112</v>
+      </c>
+      <c r="E81">
+        <v>101</v>
+      </c>
+      <c r="F81" t="s">
+        <v>134</v>
+      </c>
+      <c r="G81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>623</v>
+      </c>
+      <c r="B82" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" t="s">
+        <v>36</v>
+      </c>
+      <c r="E82">
+        <v>102</v>
+      </c>
+      <c r="F82" t="s">
+        <v>139</v>
+      </c>
+      <c r="G82" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>624</v>
+      </c>
+      <c r="B83" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" t="s">
+        <v>37</v>
+      </c>
+      <c r="E83">
+        <v>103</v>
+      </c>
+      <c r="F83" t="s">
+        <v>141</v>
+      </c>
+      <c r="G83" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>625</v>
+      </c>
+      <c r="B84" t="s">
+        <v>135</v>
+      </c>
+      <c r="C84" t="s">
         <v>115</v>
       </c>
-      <c r="C81" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>2303</v>
-      </c>
-      <c r="B82" t="s">
-        <v>110</v>
-      </c>
-      <c r="C82" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>2304</v>
-      </c>
-      <c r="B83" t="s">
-        <v>111</v>
-      </c>
-      <c r="C83" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>2305</v>
-      </c>
-      <c r="B84" t="s">
+      <c r="E84">
+        <v>104</v>
+      </c>
+      <c r="F84" t="s">
+        <v>143</v>
+      </c>
+      <c r="G84" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>626</v>
+      </c>
+      <c r="B85" t="s">
+        <v>117</v>
+      </c>
+      <c r="C85" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>627</v>
+      </c>
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>628</v>
+      </c>
+      <c r="B87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>629</v>
+      </c>
+      <c r="B88" t="s">
+        <v>129</v>
+      </c>
+      <c r="C88" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>630</v>
+      </c>
+      <c r="B89" t="s">
+        <v>137</v>
+      </c>
+      <c r="C89" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>631</v>
+      </c>
+      <c r="B90" t="s">
+        <v>120</v>
+      </c>
+      <c r="C90" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>632</v>
+      </c>
+      <c r="B91" t="s">
+        <v>121</v>
+      </c>
+      <c r="C91" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>633</v>
+      </c>
+      <c r="B92" t="s">
+        <v>122</v>
+      </c>
+      <c r="C92" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>634</v>
+      </c>
+      <c r="B93" t="s">
+        <v>136</v>
+      </c>
+      <c r="C93" t="s">
         <v>34</v>
       </c>
-      <c r="C84" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>2306</v>
-      </c>
-      <c r="B85" t="s">
-        <v>122</v>
-      </c>
-      <c r="C85" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>2307</v>
-      </c>
-      <c r="B86" t="s">
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <v>635</v>
+      </c>
+      <c r="B94" t="s">
         <v>123</v>
       </c>
-      <c r="C86" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>2308</v>
-      </c>
-      <c r="B87" t="s">
-        <v>42</v>
-      </c>
-      <c r="C87" t="s">
-        <v>95</v>
+      <c r="C94" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>636</v>
+      </c>
+      <c r="B95" t="s">
+        <v>118</v>
+      </c>
+      <c r="C95" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <v>637</v>
+      </c>
+      <c r="B96" t="s">
+        <v>124</v>
+      </c>
+      <c r="C96" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>638</v>
+      </c>
+      <c r="B97" t="s">
+        <v>131</v>
+      </c>
+      <c r="C97" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>639</v>
+      </c>
+      <c r="B98" t="s">
+        <v>132</v>
+      </c>
+      <c r="C98" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <v>640</v>
+      </c>
+      <c r="B99" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>641</v>
+      </c>
+      <c r="B100" t="s">
+        <v>139</v>
+      </c>
+      <c r="C100" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
+        <v>642</v>
+      </c>
+      <c r="B101" t="s">
+        <v>141</v>
+      </c>
+      <c r="C101" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>643</v>
+      </c>
+      <c r="B102" t="s">
+        <v>143</v>
+      </c>
+      <c r="C102" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="3">
+        <v>700</v>
+      </c>
+      <c r="B105" t="s">
+        <v>148</v>
+      </c>
+      <c r="C105" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>701</v>
+      </c>
+      <c r="B106" t="s">
+        <v>150</v>
+      </c>
+      <c r="C106" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
+        <v>702</v>
+      </c>
+      <c r="B107" t="s">
+        <v>152</v>
+      </c>
+      <c r="C107" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>703</v>
+      </c>
+      <c r="B108" t="s">
+        <v>154</v>
+      </c>
+      <c r="C108" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Partial commit while adding Program_1
</commit_message>
<xml_diff>
--- a/AssemblePrograms/Instructions Program One.xlsx
+++ b/AssemblePrograms/Instructions Program One.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManuelFrancisco\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GWU\CSCI_6461\AssemblePrograms\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -398,9 +398,6 @@
     <t>STR R1,0, POS11</t>
   </si>
   <si>
-    <t>SMR R0, 0, IX 3, 1</t>
-  </si>
-  <si>
     <t>Substract numbers</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>LDR, R0, POS 27</t>
   </si>
   <si>
-    <t>Load index to resgister 0</t>
-  </si>
-  <si>
     <t>SMR, R0, POS 19</t>
   </si>
   <si>
@@ -495,6 +489,12 @@
   </si>
   <si>
     <t>store mempost of close number</t>
+  </si>
+  <si>
+    <t>SMR R0, IX 3, 1</t>
+  </si>
+  <si>
+    <t>Load index to register 0</t>
   </si>
 </sst>
 </file>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +873,7 @@
         <v>499</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -997,7 +997,7 @@
         <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J7" t="s">
         <v>75</v>
@@ -1279,7 +1279,7 @@
         <v>522</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -1342,7 +1342,7 @@
         <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
         <v>631</v>
       </c>
       <c r="G27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>539</v>
       </c>
       <c r="B31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1742,7 +1742,7 @@
         <v>564</v>
       </c>
       <c r="B55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -1817,7 +1817,7 @@
         <v>583</v>
       </c>
       <c r="B61" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
@@ -1892,7 +1892,7 @@
         <v>603</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67" t="s">
         <v>34</v>
@@ -1948,7 +1948,7 @@
         <v>607</v>
       </c>
       <c r="B71" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C71" t="s">
         <v>34</v>
@@ -2062,7 +2062,7 @@
         <v>101</v>
       </c>
       <c r="F81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G81" t="s">
         <v>14</v>
@@ -2082,10 +2082,10 @@
         <v>102</v>
       </c>
       <c r="F82" t="s">
+        <v>138</v>
+      </c>
+      <c r="G82" t="s">
         <v>139</v>
-      </c>
-      <c r="G82" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2102,10 +2102,10 @@
         <v>103</v>
       </c>
       <c r="F83" t="s">
+        <v>140</v>
+      </c>
+      <c r="G83" t="s">
         <v>141</v>
-      </c>
-      <c r="G83" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2113,7 +2113,7 @@
         <v>625</v>
       </c>
       <c r="B84" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C84" t="s">
         <v>115</v>
@@ -2122,10 +2122,10 @@
         <v>104</v>
       </c>
       <c r="F84" t="s">
+        <v>142</v>
+      </c>
+      <c r="G84" t="s">
         <v>143</v>
-      </c>
-      <c r="G84" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
         <v>118</v>
       </c>
       <c r="C86" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2166,10 +2166,10 @@
         <v>629</v>
       </c>
       <c r="B88" t="s">
+        <v>128</v>
+      </c>
+      <c r="C88" t="s">
         <v>129</v>
-      </c>
-      <c r="C88" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,10 +2177,10 @@
         <v>630</v>
       </c>
       <c r="B89" t="s">
+        <v>136</v>
+      </c>
+      <c r="C89" t="s">
         <v>137</v>
-      </c>
-      <c r="C89" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
         <v>120</v>
       </c>
       <c r="C90" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2221,7 +2221,7 @@
         <v>634</v>
       </c>
       <c r="B93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C93" t="s">
         <v>34</v>
@@ -2254,10 +2254,10 @@
         <v>637</v>
       </c>
       <c r="B96" t="s">
+        <v>155</v>
+      </c>
+      <c r="C96" t="s">
         <v>124</v>
-      </c>
-      <c r="C96" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,10 +2265,10 @@
         <v>638</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C97" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2276,10 +2276,10 @@
         <v>639</v>
       </c>
       <c r="B98" t="s">
+        <v>131</v>
+      </c>
+      <c r="C98" t="s">
         <v>132</v>
-      </c>
-      <c r="C98" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2287,7 +2287,7 @@
         <v>640</v>
       </c>
       <c r="B99" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C99" t="s">
         <v>14</v>
@@ -2298,10 +2298,10 @@
         <v>641</v>
       </c>
       <c r="B100" t="s">
+        <v>138</v>
+      </c>
+      <c r="C100" t="s">
         <v>139</v>
-      </c>
-      <c r="C100" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2309,10 +2309,10 @@
         <v>642</v>
       </c>
       <c r="B101" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2320,10 +2320,10 @@
         <v>643</v>
       </c>
       <c r="B102" t="s">
+        <v>142</v>
+      </c>
+      <c r="C102" t="s">
         <v>143</v>
-      </c>
-      <c r="C102" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,10 +2334,10 @@
         <v>700</v>
       </c>
       <c r="B105" t="s">
+        <v>147</v>
+      </c>
+      <c r="C105" t="s">
         <v>148</v>
-      </c>
-      <c r="C105" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,10 +2345,10 @@
         <v>701</v>
       </c>
       <c r="B106" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C106" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,10 +2356,10 @@
         <v>702</v>
       </c>
       <c r="B107" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C107" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,10 +2367,10 @@
         <v>703</v>
       </c>
       <c r="B108" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C108" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JCC instruction implemented and tested and other changes.
</commit_message>
<xml_diff>
--- a/AssemblePrograms/Instructions Program One.xlsx
+++ b/AssemblePrograms/Instructions Program One.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="158">
   <si>
     <t>MEMORY ADDRESS</t>
   </si>
@@ -77,12 +77,6 @@
     <t>If not, stop</t>
   </si>
   <si>
-    <t>Is enter? (char - 13)</t>
-  </si>
-  <si>
-    <t>Is number? (char - 35)</t>
-  </si>
-  <si>
     <t>Store potential digit</t>
   </si>
   <si>
@@ -495,6 +489,15 @@
   </si>
   <si>
     <t>Load index to register 0</t>
+  </si>
+  <si>
+    <t>Is space? (char - 32)</t>
+  </si>
+  <si>
+    <t>Is number? (char - 16)</t>
+  </si>
+  <si>
+    <t>Is enter? (char - 32)</t>
   </si>
 </sst>
 </file>
@@ -832,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E80" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +876,7 @@
         <v>499</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -882,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="1">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -899,7 +902,7 @@
         <v>500</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -922,16 +925,16 @@
         <v>501</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>155</v>
       </c>
       <c r="E4">
         <v>8</v>
       </c>
       <c r="F4" s="1">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -945,10 +948,10 @@
         <v>502</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>9</v>
@@ -965,10 +968,10 @@
         <v>503</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -982,7 +985,7 @@
         <v>504</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -991,16 +994,16 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1008,10 +1011,10 @@
         <v>505</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>12</v>
@@ -1020,16 +1023,16 @@
         <v>499</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1037,25 +1040,25 @@
         <v>506</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9">
         <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1063,10 +1066,10 @@
         <v>507</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E10">
         <v>14</v>
@@ -1080,10 +1083,10 @@
         <v>508</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -1092,7 +1095,7 @@
         <v>520</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1100,16 +1103,16 @@
         <v>509</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E12">
         <v>16</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1117,10 +1120,10 @@
         <v>510</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13">
         <v>17</v>
@@ -1134,10 +1137,10 @@
         <v>511</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14">
         <v>18</v>
@@ -1146,7 +1149,7 @@
         <v>540</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1154,10 +1157,10 @@
         <v>512</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E15">
         <v>19</v>
@@ -1171,16 +1174,16 @@
         <v>513</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1191,7 +1194,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>21</v>
@@ -1200,7 +1203,7 @@
         <v>558</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1208,10 +1211,10 @@
         <v>515</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E18">
         <v>22</v>
@@ -1220,7 +1223,7 @@
         <v>539</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1231,7 +1234,7 @@
         <v>580</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1239,10 +1242,10 @@
         <v>520</v>
       </c>
       <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
         <v>31</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
       </c>
       <c r="E20">
         <v>24</v>
@@ -1251,7 +1254,7 @@
         <v>600</v>
       </c>
       <c r="G20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1259,10 +1262,10 @@
         <v>521</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21">
         <v>25</v>
@@ -1271,7 +1274,7 @@
         <v>560</v>
       </c>
       <c r="G21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1279,10 +1282,10 @@
         <v>522</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22">
         <v>26</v>
@@ -1296,16 +1299,16 @@
         <v>523</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E23">
         <v>27</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1313,10 +1316,10 @@
         <v>524</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E24">
         <v>28</v>
@@ -1325,7 +1328,7 @@
         <v>620</v>
       </c>
       <c r="G24" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1333,16 +1336,16 @@
         <v>525</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E25">
         <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1350,10 +1353,10 @@
         <v>526</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E26">
         <v>30</v>
@@ -1362,7 +1365,7 @@
         <v>700</v>
       </c>
       <c r="G26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1370,10 +1373,10 @@
         <v>527</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E27">
         <v>31</v>
@@ -1382,7 +1385,7 @@
         <v>631</v>
       </c>
       <c r="G27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1390,10 +1393,10 @@
         <v>528</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1401,10 +1404,10 @@
         <v>529</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1412,7 +1415,7 @@
         <v>539</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1429,7 +1432,7 @@
         <v>540</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
@@ -1446,10 +1449,10 @@
         <v>541</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="E33">
         <v>1002</v>
@@ -1460,10 +1463,10 @@
         <v>542</v>
       </c>
       <c r="B34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E34">
         <v>1003</v>
@@ -1474,10 +1477,10 @@
         <v>543</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
       <c r="E35">
         <v>1004</v>
@@ -1488,7 +1491,7 @@
         <v>544</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
@@ -1502,10 +1505,10 @@
         <v>545</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E37">
         <v>1006</v>
@@ -1516,10 +1519,10 @@
         <v>546</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E38">
         <v>1007</v>
@@ -1530,10 +1533,10 @@
         <v>547</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E39">
         <v>1008</v>
@@ -1544,10 +1547,10 @@
         <v>548</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E40">
         <v>1009</v>
@@ -1558,10 +1561,10 @@
         <v>549</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E41">
         <v>1010</v>
@@ -1572,10 +1575,10 @@
         <v>550</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E42">
         <v>1011</v>
@@ -1586,10 +1589,10 @@
         <v>551</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E43">
         <v>1012</v>
@@ -1600,10 +1603,10 @@
         <v>552</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C44" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E44">
         <v>1013</v>
@@ -1614,10 +1617,10 @@
         <v>553</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E45">
         <v>1014</v>
@@ -1631,7 +1634,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E46">
         <v>1015</v>
@@ -1642,10 +1645,10 @@
         <v>555</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E47">
         <v>1016</v>
@@ -1661,10 +1664,10 @@
         <v>558</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E49">
         <v>1018</v>
@@ -1675,10 +1678,10 @@
         <v>559</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C50" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E50">
         <v>1019</v>
@@ -1689,10 +1692,10 @@
         <v>560</v>
       </c>
       <c r="B51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E51">
         <v>1020</v>
@@ -1703,10 +1706,10 @@
         <v>561</v>
       </c>
       <c r="B52" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" t="s">
         <v>78</v>
-      </c>
-      <c r="C52" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1714,10 +1717,10 @@
         <v>562</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E53">
         <v>1501</v>
@@ -1728,10 +1731,10 @@
         <v>563</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E54">
         <v>1502</v>
@@ -1742,7 +1745,7 @@
         <v>564</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -1756,10 +1759,10 @@
         <v>565</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E56">
         <v>1504</v>
@@ -1775,10 +1778,10 @@
         <v>580</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E58">
         <v>1506</v>
@@ -1789,10 +1792,10 @@
         <v>581</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E59">
         <v>1507</v>
@@ -1803,10 +1806,10 @@
         <v>582</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E60">
         <v>1508</v>
@@ -1817,7 +1820,7 @@
         <v>583</v>
       </c>
       <c r="B61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
@@ -1831,10 +1834,10 @@
         <v>584</v>
       </c>
       <c r="B62" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C62" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E62">
         <v>1510</v>
@@ -1850,10 +1853,10 @@
         <v>600</v>
       </c>
       <c r="B64" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" t="s">
         <v>100</v>
-      </c>
-      <c r="C64" t="s">
-        <v>102</v>
       </c>
       <c r="E64">
         <v>1512</v>
@@ -1864,10 +1867,10 @@
         <v>601</v>
       </c>
       <c r="B65" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E65">
         <v>1513</v>
@@ -1878,10 +1881,10 @@
         <v>602</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C66" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E66">
         <v>1514</v>
@@ -1892,10 +1895,10 @@
         <v>603</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C67" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E67">
         <v>1515</v>
@@ -1906,10 +1909,10 @@
         <v>604</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C68" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E68">
         <v>1516</v>
@@ -1920,10 +1923,10 @@
         <v>605</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C69" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E69">
         <v>1517</v>
@@ -1934,10 +1937,10 @@
         <v>606</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C70" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E70">
         <v>1518</v>
@@ -1948,10 +1951,10 @@
         <v>607</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E71">
         <v>1519</v>
@@ -1962,10 +1965,10 @@
         <v>608</v>
       </c>
       <c r="B72" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C72" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E72">
         <v>1520</v>
@@ -1976,10 +1979,10 @@
         <v>609</v>
       </c>
       <c r="B73" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C73" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1987,10 +1990,10 @@
         <v>610</v>
       </c>
       <c r="B74" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1998,10 +2001,10 @@
         <v>611</v>
       </c>
       <c r="B75" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C75" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2009,10 +2012,10 @@
         <v>612</v>
       </c>
       <c r="B76" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C76" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2020,10 +2023,10 @@
         <v>613</v>
       </c>
       <c r="B77" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2031,10 +2034,10 @@
         <v>620</v>
       </c>
       <c r="B79" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C79" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2042,10 +2045,10 @@
         <v>621</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2053,16 +2056,16 @@
         <v>622</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C81" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E81">
         <v>101</v>
       </c>
       <c r="F81" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G81" t="s">
         <v>14</v>
@@ -2073,19 +2076,19 @@
         <v>623</v>
       </c>
       <c r="B82" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C82" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E82">
         <v>102</v>
       </c>
       <c r="F82" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G82" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2093,19 +2096,19 @@
         <v>624</v>
       </c>
       <c r="B83" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C83" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E83">
         <v>103</v>
       </c>
       <c r="F83" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G83" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2113,19 +2116,19 @@
         <v>625</v>
       </c>
       <c r="B84" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C84" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E84">
         <v>104</v>
       </c>
       <c r="F84" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G84" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2133,10 +2136,10 @@
         <v>626</v>
       </c>
       <c r="B85" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C85" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2144,10 +2147,10 @@
         <v>627</v>
       </c>
       <c r="B86" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C86" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2155,10 +2158,10 @@
         <v>628</v>
       </c>
       <c r="B87" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C87" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2166,10 +2169,10 @@
         <v>629</v>
       </c>
       <c r="B88" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C88" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,10 +2180,10 @@
         <v>630</v>
       </c>
       <c r="B89" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C89" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2188,10 +2191,10 @@
         <v>631</v>
       </c>
       <c r="B90" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C90" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2199,10 +2202,10 @@
         <v>632</v>
       </c>
       <c r="B91" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C91" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -2210,10 +2213,10 @@
         <v>633</v>
       </c>
       <c r="B92" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C92" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2221,10 +2224,10 @@
         <v>634</v>
       </c>
       <c r="B93" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C93" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -2232,10 +2235,10 @@
         <v>635</v>
       </c>
       <c r="B94" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C94" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2243,10 +2246,10 @@
         <v>636</v>
       </c>
       <c r="B95" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C95" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2254,10 +2257,10 @@
         <v>637</v>
       </c>
       <c r="B96" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C96" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2265,10 +2268,10 @@
         <v>638</v>
       </c>
       <c r="B97" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C97" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2276,10 +2279,10 @@
         <v>639</v>
       </c>
       <c r="B98" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C98" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2287,7 +2290,7 @@
         <v>640</v>
       </c>
       <c r="B99" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C99" t="s">
         <v>14</v>
@@ -2298,10 +2301,10 @@
         <v>641</v>
       </c>
       <c r="B100" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C100" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2309,10 +2312,10 @@
         <v>642</v>
       </c>
       <c r="B101" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C101" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2320,10 +2323,10 @@
         <v>643</v>
       </c>
       <c r="B102" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C102" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,10 +2337,10 @@
         <v>700</v>
       </c>
       <c r="B105" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C105" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,10 +2348,10 @@
         <v>701</v>
       </c>
       <c r="B106" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C106" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,10 +2359,10 @@
         <v>702</v>
       </c>
       <c r="B107" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C107" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,10 +2370,10 @@
         <v>703</v>
       </c>
       <c r="B108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C108" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More little changes to make program 1 work.
</commit_message>
<xml_diff>
--- a/AssemblePrograms/Instructions Program One.xlsx
+++ b/AssemblePrograms/Instructions Program One.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="157">
   <si>
     <t>MEMORY ADDRESS</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Store number</t>
   </si>
   <si>
-    <t>If it is enter, go to routine to IX 1 ++</t>
-  </si>
-  <si>
     <t>STX IX 1, POS16</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
     <t>JCC CC(1), 0, POS 7, 1</t>
   </si>
   <si>
-    <t>JCC CC(1), 0, POS 15,1</t>
-  </si>
-  <si>
     <t>JCC CC(1), 0, POS 11,1</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>STR R1, 0, 20</t>
   </si>
   <si>
-    <t>JCC CC(1), 0, POS 21,1</t>
-  </si>
-  <si>
     <t>before start phase 1</t>
   </si>
   <si>
@@ -257,9 +248,6 @@
     <t>SMR R0, 0, POS20</t>
   </si>
   <si>
-    <t>If it is enter, go to routine to search in 2200</t>
-  </si>
-  <si>
     <t>Substract number and search number</t>
   </si>
   <si>
@@ -497,7 +485,16 @@
     <t>Is number? (char - 16)</t>
   </si>
   <si>
-    <t>Is enter? (char - 32)</t>
+    <t>If it is space, go to routine to IX 1 ++</t>
+  </si>
+  <si>
+    <t>JZ, R2, 0,POS 15,1</t>
+  </si>
+  <si>
+    <t>JZ, R2, 0,POS 21,1</t>
+  </si>
+  <si>
+    <t>If it is space, go to routine to search in 558</t>
   </si>
 </sst>
 </file>
@@ -835,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,7 +873,7 @@
         <v>499</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -928,7 +925,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E4">
         <v>8</v>
@@ -948,10 +945,10 @@
         <v>502</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>153</v>
       </c>
       <c r="E5">
         <v>9</v>
@@ -971,7 +968,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -985,7 +982,7 @@
         <v>504</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -994,16 +991,16 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1023,16 +1020,16 @@
         <v>499</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1040,25 +1037,25 @@
         <v>506</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9">
         <v>13</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H9" t="s">
         <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1066,10 +1063,10 @@
         <v>507</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E10">
         <v>14</v>
@@ -1083,10 +1080,10 @@
         <v>508</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -1095,7 +1092,7 @@
         <v>520</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1103,16 +1100,16 @@
         <v>509</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12">
         <v>16</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1137,10 +1134,10 @@
         <v>511</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14">
         <v>18</v>
@@ -1149,7 +1146,7 @@
         <v>540</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1174,7 +1171,7 @@
         <v>513</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -1183,7 +1180,7 @@
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1203,7 +1200,7 @@
         <v>558</v>
       </c>
       <c r="G17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1211,10 +1208,10 @@
         <v>515</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E18">
         <v>22</v>
@@ -1223,7 +1220,7 @@
         <v>539</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1234,7 +1231,7 @@
         <v>580</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1242,10 +1239,10 @@
         <v>520</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20">
         <v>24</v>
@@ -1254,7 +1251,7 @@
         <v>600</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1262,10 +1259,10 @@
         <v>521</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>25</v>
@@ -1274,7 +1271,7 @@
         <v>560</v>
       </c>
       <c r="G21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1282,10 +1279,10 @@
         <v>522</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22">
         <v>26</v>
@@ -1299,16 +1296,16 @@
         <v>523</v>
       </c>
       <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
         <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>34</v>
       </c>
       <c r="E23">
         <v>27</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1316,10 +1313,10 @@
         <v>524</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24">
         <v>28</v>
@@ -1328,7 +1325,7 @@
         <v>620</v>
       </c>
       <c r="G24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1336,16 +1333,16 @@
         <v>525</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25">
         <v>29</v>
       </c>
       <c r="F25" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1353,10 +1350,10 @@
         <v>526</v>
       </c>
       <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
         <v>40</v>
-      </c>
-      <c r="C26" t="s">
-        <v>41</v>
       </c>
       <c r="E26">
         <v>30</v>
@@ -1365,7 +1362,7 @@
         <v>700</v>
       </c>
       <c r="G26" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1373,10 +1370,10 @@
         <v>527</v>
       </c>
       <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
         <v>42</v>
-      </c>
-      <c r="C27" t="s">
-        <v>43</v>
       </c>
       <c r="E27">
         <v>31</v>
@@ -1385,7 +1382,7 @@
         <v>631</v>
       </c>
       <c r="G27" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1393,10 +1390,10 @@
         <v>528</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1404,10 +1401,10 @@
         <v>529</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1415,7 +1412,7 @@
         <v>539</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -1452,7 +1449,7 @@
         <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E33">
         <v>1002</v>
@@ -1463,10 +1460,10 @@
         <v>542</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="E34">
         <v>1003</v>
@@ -1480,7 +1477,7 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E35">
         <v>1004</v>
@@ -1491,7 +1488,7 @@
         <v>544</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" t="s">
         <v>16</v>
@@ -1519,10 +1516,10 @@
         <v>546</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E38">
         <v>1007</v>
@@ -1533,10 +1530,10 @@
         <v>547</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E39">
         <v>1008</v>
@@ -1547,10 +1544,10 @@
         <v>548</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E40">
         <v>1009</v>
@@ -1561,10 +1558,10 @@
         <v>549</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E41">
         <v>1010</v>
@@ -1575,7 +1572,7 @@
         <v>550</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
@@ -1589,10 +1586,10 @@
         <v>551</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E43">
         <v>1012</v>
@@ -1617,7 +1614,7 @@
         <v>553</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
         <v>19</v>
@@ -1645,10 +1642,10 @@
         <v>555</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E47">
         <v>1016</v>
@@ -1664,10 +1661,10 @@
         <v>558</v>
       </c>
       <c r="B49" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E49">
         <v>1018</v>
@@ -1678,10 +1675,10 @@
         <v>559</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E50">
         <v>1019</v>
@@ -1692,10 +1689,10 @@
         <v>560</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E51">
         <v>1020</v>
@@ -1706,10 +1703,10 @@
         <v>561</v>
       </c>
       <c r="B52" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1717,10 +1714,10 @@
         <v>562</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E53">
         <v>1501</v>
@@ -1731,10 +1728,10 @@
         <v>563</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C54" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E54">
         <v>1502</v>
@@ -1745,7 +1742,7 @@
         <v>564</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C55" t="s">
         <v>14</v>
@@ -1759,10 +1756,10 @@
         <v>565</v>
       </c>
       <c r="B56" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E56">
         <v>1504</v>
@@ -1778,10 +1775,10 @@
         <v>580</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E58">
         <v>1506</v>
@@ -1792,10 +1789,10 @@
         <v>581</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E59">
         <v>1507</v>
@@ -1806,10 +1803,10 @@
         <v>582</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E60">
         <v>1508</v>
@@ -1820,7 +1817,7 @@
         <v>583</v>
       </c>
       <c r="B61" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C61" t="s">
         <v>14</v>
@@ -1834,10 +1831,10 @@
         <v>584</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C62" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E62">
         <v>1510</v>
@@ -1853,10 +1850,10 @@
         <v>600</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C64" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E64">
         <v>1512</v>
@@ -1867,10 +1864,10 @@
         <v>601</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C65" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E65">
         <v>1513</v>
@@ -1881,10 +1878,10 @@
         <v>602</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C66" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E66">
         <v>1514</v>
@@ -1895,10 +1892,10 @@
         <v>603</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E67">
         <v>1515</v>
@@ -1909,10 +1906,10 @@
         <v>604</v>
       </c>
       <c r="B68" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E68">
         <v>1516</v>
@@ -1923,10 +1920,10 @@
         <v>605</v>
       </c>
       <c r="B69" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E69">
         <v>1517</v>
@@ -1937,10 +1934,10 @@
         <v>606</v>
       </c>
       <c r="B70" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C70" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E70">
         <v>1518</v>
@@ -1951,10 +1948,10 @@
         <v>607</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E71">
         <v>1519</v>
@@ -1965,10 +1962,10 @@
         <v>608</v>
       </c>
       <c r="B72" t="s">
+        <v>32</v>
+      </c>
+      <c r="C72" t="s">
         <v>33</v>
-      </c>
-      <c r="C72" t="s">
-        <v>34</v>
       </c>
       <c r="E72">
         <v>1520</v>
@@ -1979,10 +1976,10 @@
         <v>609</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1990,10 +1987,10 @@
         <v>610</v>
       </c>
       <c r="B74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C74" t="s">
         <v>40</v>
-      </c>
-      <c r="C74" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2001,10 +1998,10 @@
         <v>611</v>
       </c>
       <c r="B75" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75" t="s">
         <v>42</v>
-      </c>
-      <c r="C75" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,10 +2009,10 @@
         <v>612</v>
       </c>
       <c r="B76" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C76" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2023,10 +2020,10 @@
         <v>613</v>
       </c>
       <c r="B77" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C77" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2034,10 +2031,10 @@
         <v>620</v>
       </c>
       <c r="B79" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C79" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2045,10 +2042,10 @@
         <v>621</v>
       </c>
       <c r="B80" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2056,16 +2053,16 @@
         <v>622</v>
       </c>
       <c r="B81" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C81" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E81">
         <v>101</v>
       </c>
       <c r="F81" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G81" t="s">
         <v>14</v>
@@ -2076,19 +2073,19 @@
         <v>623</v>
       </c>
       <c r="B82" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C82" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E82">
         <v>102</v>
       </c>
       <c r="F82" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G82" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2096,19 +2093,19 @@
         <v>624</v>
       </c>
       <c r="B83" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C83" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E83">
         <v>103</v>
       </c>
       <c r="F83" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G83" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2116,19 +2113,19 @@
         <v>625</v>
       </c>
       <c r="B84" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C84" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E84">
         <v>104</v>
       </c>
       <c r="F84" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G84" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2136,10 +2133,10 @@
         <v>626</v>
       </c>
       <c r="B85" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C85" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2147,10 +2144,10 @@
         <v>627</v>
       </c>
       <c r="B86" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C86" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2158,10 +2155,10 @@
         <v>628</v>
       </c>
       <c r="B87" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C87" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2169,10 +2166,10 @@
         <v>629</v>
       </c>
       <c r="B88" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C88" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2180,10 +2177,10 @@
         <v>630</v>
       </c>
       <c r="B89" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C89" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2191,10 +2188,10 @@
         <v>631</v>
       </c>
       <c r="B90" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C90" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2202,10 +2199,10 @@
         <v>632</v>
       </c>
       <c r="B91" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C91" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -2213,10 +2210,10 @@
         <v>633</v>
       </c>
       <c r="B92" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C92" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2224,10 +2221,10 @@
         <v>634</v>
       </c>
       <c r="B93" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C93" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -2235,10 +2232,10 @@
         <v>635</v>
       </c>
       <c r="B94" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C94" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -2246,10 +2243,10 @@
         <v>636</v>
       </c>
       <c r="B95" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C95" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2257,10 +2254,10 @@
         <v>637</v>
       </c>
       <c r="B96" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C96" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,10 +2265,10 @@
         <v>638</v>
       </c>
       <c r="B97" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C97" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,10 +2276,10 @@
         <v>639</v>
       </c>
       <c r="B98" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C98" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2287,7 @@
         <v>640</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C99" t="s">
         <v>14</v>
@@ -2301,10 +2298,10 @@
         <v>641</v>
       </c>
       <c r="B100" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C100" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,10 +2309,10 @@
         <v>642</v>
       </c>
       <c r="B101" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C101" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,10 +2320,10 @@
         <v>643</v>
       </c>
       <c r="B102" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C102" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2337,10 +2334,10 @@
         <v>700</v>
       </c>
       <c r="B105" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C105" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2348,10 +2345,10 @@
         <v>701</v>
       </c>
       <c r="B106" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C106" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2359,10 +2356,10 @@
         <v>702</v>
       </c>
       <c r="B107" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C107" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2370,10 +2367,10 @@
         <v>703</v>
       </c>
       <c r="B108" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C108" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>